<commit_message>
Rettelse i forhold til review
</commit_message>
<xml_diff>
--- a/05 Test/ATD10 Brug login.xlsx
+++ b/05 Test/ATD10 Brug login.xlsx
@@ -70,7 +70,7 @@
     <t xml:space="preserve">TC5</t>
   </si>
   <si>
-    <t xml:space="preserve">Ingen internetforbindelse</t>
+    <t xml:space="preserve">Ingen internetforbindelse ved først login</t>
   </si>
   <si>
     <t xml:space="preserve">Fejl: Begrænset eller ingen internetadgang</t>
@@ -351,7 +351,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>